<commit_message>
Adds data to the spreadsheet
</commit_message>
<xml_diff>
--- a/LostAndFound/LostAndFound/Resources/LostAndFound.xlsx
+++ b/LostAndFound/LostAndFound/Resources/LostAndFound.xlsx
@@ -21,6 +21,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +368,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified and created the Excel spreadsheets
</commit_message>
<xml_diff>
--- a/LostAndFound/LostAndFound/Resources/LostAndFound.xlsx
+++ b/LostAndFound/LostAndFound/Resources/LostAndFound.xlsx
@@ -418,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A7" sqref="A7:XFD7"/>
@@ -557,6 +557,57 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>JERSH</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>MERXWERLS</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>123-111-9928</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>JERSH</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>MERXWERLS</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>123-111-9928</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>JERSH</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>MERXWERLS</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>123-111-9928</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
Item Providers Part Deux
Hopefully Works??!?!?!?
</commit_message>
<xml_diff>
--- a/LostAndFound/LostAndFound/Resources/LostAndFound.xlsx
+++ b/LostAndFound/LostAndFound/Resources/LostAndFound.xlsx
@@ -418,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A7" sqref="A7:XFD7"/>
@@ -485,17 +485,23 @@
       </c>
     </row>
     <row spans="1:5" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>JESSAy</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>maerxhwelrl</t>
+        </is>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>123-456-8678</t>
+        </is>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -603,6 +609,23 @@
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>123-111-9928</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>JERSH</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>MERXWERLS</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>123-111-9928</t>
         </is>

</xml_diff>